<commit_message>
SE-2801: Removed 'source' assignment in txn config setup
</commit_message>
<xml_diff>
--- a/examples/use-cases/ibor/data/transaction_type_consolidation_data.xlsx
+++ b/examples/use-cases/ibor/data/transaction_type_consolidation_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasPartridge\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\sample-notebooks\examples\use-cases\ibor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48F62BB-F7C4-4667-9106-EF629FA1B8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81542D2-0A8C-4E73-A58E-EDBAEB27E7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="-11970" windowWidth="21600" windowHeight="11325" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="3" r:id="rId1"/>
@@ -127,18 +127,6 @@
     <t>BuyL</t>
   </si>
   <si>
-    <t>txnid_SSCust0001</t>
-  </si>
-  <si>
-    <t>txnid_SSCust0002</t>
-  </si>
-  <si>
-    <t>txnid_BNPCust0001</t>
-  </si>
-  <si>
-    <t>txnid_BNPCust0002</t>
-  </si>
-  <si>
     <t>txn_source</t>
   </si>
   <si>
@@ -214,12 +202,6 @@
     <t>txnid_OMS0004</t>
   </si>
   <si>
-    <t>txnid_SSCust0003</t>
-  </si>
-  <si>
-    <t>txnid_BNPCust0003</t>
-  </si>
-  <si>
     <t>EnergyFundUS</t>
   </si>
   <si>
@@ -233,6 +215,24 @@
   </si>
   <si>
     <t>EnergyFundAmericasExUS</t>
+  </si>
+  <si>
+    <t>txnid_USCust0001</t>
+  </si>
+  <si>
+    <t>txnid_USCust0002</t>
+  </si>
+  <si>
+    <t>txnid_USCust0003</t>
+  </si>
+  <si>
+    <t>txnid_FRCust0001</t>
+  </si>
+  <si>
+    <t>txnid_FRCust0002</t>
+  </si>
+  <si>
+    <t>txnid_FRCust0003</t>
   </si>
 </sst>
 </file>
@@ -621,26 +621,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E4483A-D81C-486B-9469-6BB1913F7014}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -657,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
@@ -675,12 +675,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>28</v>
@@ -692,7 +692,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>20</v>
@@ -710,12 +710,12 @@
         <v>665000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>28</v>
@@ -727,7 +727,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>20</v>
@@ -745,24 +745,24 @@
         <v>625000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>20</v>
@@ -780,24 +780,24 @@
         <v>647500</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>20</v>
@@ -815,12 +815,12 @@
         <v>660000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>29</v>
@@ -832,7 +832,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>20</v>
@@ -850,24 +850,24 @@
         <v>495000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>20</v>
@@ -885,24 +885,24 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
         <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>20</v>
@@ -920,24 +920,24 @@
         <v>495000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3">
         <v>101</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>20</v>
@@ -955,24 +955,24 @@
         <v>337500</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3">
         <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>20</v>
@@ -990,24 +990,24 @@
         <v>325000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3">
         <v>101</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>20</v>
@@ -1025,19 +1025,19 @@
         <v>330000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K14" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="5"/>
     </row>
   </sheetData>
@@ -1055,15 +1055,15 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1105,35 +1105,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1147,74 +1147,74 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="D11" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>